<commit_message>
this verison make patient drug seq data is built after first diagnosis day
</commit_message>
<xml_diff>
--- a/data/resultTmp/fisherscoreSimpleVerify.xlsx
+++ b/data/resultTmp/fisherscoreSimpleVerify.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="192" windowWidth="19140" windowHeight="10788"/>
+    <workbookView xWindow="5460" yWindow="1880" windowWidth="28760" windowHeight="16240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>f1</t>
   </si>
@@ -55,17 +60,47 @@
   </si>
   <si>
     <t>This simple example is used to verify the fisher score function. Code existed in demo/src/test/java/spmFuncTest/.java fisherscoreTest function.</t>
+  </si>
+  <si>
+    <t>Fscore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -87,14 +122,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="9">
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="7" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -395,17 +446,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -434,78 +485,78 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1.2</v>
       </c>
       <c r="F2">
         <f>C2-E2</f>
-        <v>0.8</v>
+        <v>-0.19999999999999996</v>
       </c>
       <c r="G2">
         <f>F2*F2</f>
-        <v>0.64000000000000012</v>
+        <v>3.999999999999998E-2</v>
       </c>
       <c r="H2">
         <v>0.4</v>
       </c>
       <c r="I2">
         <f>D2-H2</f>
-        <v>1.6</v>
+        <v>0.6</v>
       </c>
       <c r="J2">
         <f>I2^2</f>
-        <v>2.5600000000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1.2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F11" si="0">C3-E3</f>
-        <v>0.8</v>
+        <f t="shared" ref="F3:F6" si="0">C3-E3</f>
+        <v>-1.2</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G6" si="1">F3*F3</f>
-        <v>0.64000000000000012</v>
+        <v>1.44</v>
       </c>
       <c r="H3">
         <v>0.4</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I6" si="2">D3-H3</f>
-        <v>-0.4</v>
+        <v>0.6</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J6" si="3">I3^2</f>
-        <v>0.16000000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -515,11 +566,11 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>0.64000000000000012</v>
+        <v>1.44</v>
       </c>
       <c r="H4">
         <v>0.4</v>
@@ -533,7 +584,7 @@
         <v>0.16000000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="B5">
         <v>0</v>
       </c>
@@ -566,7 +617,7 @@
         <v>0.16000000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6">
         <v>0</v>
       </c>
@@ -599,83 +650,83 @@
         <v>0.16000000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f>SUM(G2:G6)/5</f>
-        <v>0.96000000000000019</v>
+        <v>1.1599999999999997</v>
       </c>
       <c r="J7">
         <f>AVERAGE(J2:J6)</f>
-        <v>0.64000000000000024</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.24000000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="C12">
         <f>AVERAGE(C2:C11)</f>
-        <v>1.6</v>
+        <v>0.6</v>
       </c>
       <c r="D12">
         <f>AVERAGE(D2:D11)</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>0</v>
       </c>
@@ -684,14 +735,14 @@
       </c>
       <c r="C13">
         <f>AVERAGE(C2:C6)</f>
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="D13">
         <f>AVERAGE(D2:D6)</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>1</v>
       </c>
@@ -700,40 +751,67 @@
       </c>
       <c r="C14">
         <f>AVERAGE(C7:C11)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f>AVERAGE(D7:D11)</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>0</v>
       </c>
       <c r="C15">
         <f>((C13-C12)^2)*B13</f>
-        <v>0.8000000000000006</v>
+        <v>0.79999999999999982</v>
       </c>
       <c r="D15">
         <f>((D13-D12)^2)*B13</f>
-        <v>0.1999999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.9999999999999975E-2</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="C16">
         <f>((C14-C12)^2)*B14</f>
-        <v>0.7999999999999996</v>
+        <v>0.80000000000000016</v>
       </c>
       <c r="D16">
         <f>((D14-D12)^2)*B14</f>
-        <v>0.20000000000000015</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.9999999999999975E-2</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -743,10 +821,19 @@
       </c>
       <c r="D17">
         <f>SUM(D15:D16)</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9.999999999999995E-2</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>0</v>
       </c>
@@ -755,14 +842,23 @@
       </c>
       <c r="C18">
         <f>_xlfn.VAR.P(C2:C6)</f>
-        <v>0.96</v>
+        <v>0.16</v>
       </c>
       <c r="D18">
         <f>_xlfn.VAR.P(D2:D6)</f>
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.24</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>1</v>
       </c>
@@ -775,23 +871,41 @@
       </c>
       <c r="D19">
         <f>_xlfn.VAR.P(D7:D11)</f>
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.24</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>0</v>
       </c>
       <c r="C20">
         <f>B18*C18</f>
-        <v>4.8</v>
+        <v>0.8</v>
       </c>
       <c r="D20">
         <f>B18*D18</f>
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.2</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>1</v>
       </c>
@@ -801,47 +915,103 @@
       </c>
       <c r="D21">
         <f>B19*D19</f>
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.2</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22">
         <f>SUM(C20:C21)</f>
-        <v>4.8</v>
+        <v>0.8</v>
       </c>
       <c r="D22">
         <f>SUM(D20:D21)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.4</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23">
         <f>C17/C22</f>
-        <v>0.33333333333333337</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <f>D17/D22</f>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.166666666666665E-2</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="H25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -851,9 +1021,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -863,8 +1039,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>